<commit_message>
Framework and OPS changes
</commit_message>
<xml_diff>
--- a/SRFROWCA/TEST/Chad.xlsx
+++ b/SRFROWCA/TEST/Chad.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
   <si>
     <t>Objective</t>
   </si>
@@ -269,6 +269,72 @@
   </si>
   <si>
     <t>ors@ocharowca.info</t>
+  </si>
+  <si>
+    <t>Barh El Gazel</t>
+  </si>
+  <si>
+    <t>Batha</t>
+  </si>
+  <si>
+    <t>Borkou</t>
+  </si>
+  <si>
+    <t>Chari Baguirmi</t>
+  </si>
+  <si>
+    <t>Ennedi</t>
+  </si>
+  <si>
+    <t>Guera</t>
+  </si>
+  <si>
+    <t>Hadjer Lamis</t>
+  </si>
+  <si>
+    <t>Kanem</t>
+  </si>
+  <si>
+    <t>Lac</t>
+  </si>
+  <si>
+    <t>Logone Occidental</t>
+  </si>
+  <si>
+    <t>Logone Oriental</t>
+  </si>
+  <si>
+    <t>Mandoul</t>
+  </si>
+  <si>
+    <t>Mayo Kebbi Est</t>
+  </si>
+  <si>
+    <t>Mayo Kebbi Ouest</t>
+  </si>
+  <si>
+    <t>Moyen Chari</t>
+  </si>
+  <si>
+    <t>N'Djamena</t>
+  </si>
+  <si>
+    <t>Ouaddai</t>
+  </si>
+  <si>
+    <t>Salamat</t>
+  </si>
+  <si>
+    <t>Sila</t>
+  </si>
+  <si>
+    <t>Tandjile</t>
+  </si>
+  <si>
+    <t>Tibesti</t>
+  </si>
+  <si>
+    <t>Wadi Fira</t>
   </si>
 </sst>
 </file>
@@ -388,16 +454,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -737,7 +797,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -750,82 +810,105 @@
     <col min="5" max="5" width="33.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="H1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -847,285 +930,285 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
     </row>
     <row r="4" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-      <c r="P10" s="19"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-      <c r="P12" s="19"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
     </row>
     <row r="15" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="11"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1163,278 +1246,278 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:16" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
     </row>
     <row r="3" spans="1:16" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="19"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="19"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-      <c r="P9" s="19"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
     </row>
     <row r="15" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="9"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>